<commit_message>
impute missing data, CV and LB worse
</commit_message>
<xml_diff>
--- a/Kaggle Safe_Driver_Prediction 调试过程记录.xlsx
+++ b/Kaggle Safe_Driver_Prediction 调试过程记录.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
   <si>
     <t>Sub Datas</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>simple xgb-cv baseline</t>
+  </si>
+  <si>
+    <t>简单填充所有缺失值</t>
   </si>
 </sst>
 </file>
@@ -100,7 +103,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,6 +119,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="44"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,7 +164,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -186,10 +195,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -533,19 +545,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="23.275" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.91666666666667" style="3" customWidth="1"/>
+    <col min="2" max="2" width="7.68333333333333" style="3" customWidth="1"/>
     <col min="3" max="3" width="18.55" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.775" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.925" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.5583333333333" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.4166666666667" style="3" customWidth="1"/>
     <col min="6" max="10" width="13.35" style="3" customWidth="1"/>
     <col min="11" max="11" width="16.775" style="3" customWidth="1"/>
     <col min="12" max="12" width="14.5" style="3" customWidth="1"/>
@@ -562,14 +574,14 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" s="1" customFormat="1" ht="31" customHeight="1" spans="1:14">
       <c r="A2" s="7" t="s">
@@ -634,15 +646,58 @@
       <c r="F3" s="9">
         <v>0.23295148883</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="G3" s="9">
+        <v>0.0340517160894</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0.0348116346456</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0.418398802664</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0.272740663109</v>
+      </c>
+      <c r="K3" s="9">
+        <v>0.266</v>
+      </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:1">
-      <c r="A4" s="10"/>
+    <row r="4" ht="25" customHeight="1" spans="1:10">
+      <c r="A4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="11">
+        <v>57</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.0629465602144</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.0637251145801</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.385213390555</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.213319329447</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0.0340311075112</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.0348125245684</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.411609902773</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0.271547618074</v>
+      </c>
     </row>
+    <row r="5" ht="25" customHeight="1"/>
+    <row r="6" ht="25" customHeight="1"/>
+    <row r="7" ht="20" customHeight="1"/>
+    <row r="8" ht="28" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:F1"/>

</xml_diff>